<commit_message>
fixing small error in question 1
</commit_message>
<xml_diff>
--- a/projet-EXEL.xlsx
+++ b/projet-EXEL.xlsx
@@ -1,32 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lilia\Desktop\try\projet-final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\OneDrive\Desktop\projet-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B817D8F-F758-4B41-996D-A7CA2D43927E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0092323-0D6F-4028-926E-A01146FF9E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="4" xr2:uid="{F862E75D-BEDF-4E7C-832F-4D36265961D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{F862E75D-BEDF-4E7C-832F-4D36265961D6}"/>
   </bookViews>
   <sheets>
-    <sheet name="table1" sheetId="2" r:id="rId1"/>
-    <sheet name="Table2" sheetId="5" r:id="rId2"/>
-    <sheet name="Table3" sheetId="6" r:id="rId3"/>
-    <sheet name="Question3" sheetId="7" r:id="rId4"/>
-    <sheet name="Question4" sheetId="8" r:id="rId5"/>
-    <sheet name="Qustion 1" sheetId="1" r:id="rId6"/>
+    <sheet name="Question1" sheetId="10" r:id="rId1"/>
+    <sheet name="Table1" sheetId="11" r:id="rId2"/>
+    <sheet name="Table2" sheetId="12" r:id="rId3"/>
+    <sheet name="Table3" sheetId="13" r:id="rId4"/>
+    <sheet name="Question3" sheetId="7" r:id="rId5"/>
+    <sheet name="Question4" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId7"/>
+    <pivotCache cacheId="12" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -65,13 +74,7 @@
     <t>Cornell</t>
   </si>
   <si>
-    <t>Colombia</t>
-  </si>
-  <si>
     <t>Princeton</t>
-  </si>
-  <si>
-    <t>Penn state</t>
   </si>
   <si>
     <t>Ivy League Applicants</t>
@@ -84,21 +87,6 @@
   </si>
   <si>
     <t>University</t>
-  </si>
-  <si>
-    <t>Étiquettes de lignes</t>
-  </si>
-  <si>
-    <t>Total général</t>
-  </si>
-  <si>
-    <t>Somme de Students</t>
-  </si>
-  <si>
-    <t>Étiquettes de colonnes</t>
-  </si>
-  <si>
-    <t>Moyenne de Students2</t>
   </si>
   <si>
     <t>ID</t>
@@ -142,17 +130,37 @@
   <si>
     <t>TTC:</t>
   </si>
+  <si>
+    <t>Columbia</t>
+  </si>
+  <si>
+    <t>Penn</t>
+  </si>
+  <si>
+    <t>Sum of Students</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Average of Students2</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00\ [$DZD]"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00\ [$DZD]"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +179,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,12 +212,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -210,6 +219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,32 +281,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -301,49 +299,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -359,7 +374,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -858,7 +873,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2561,9 +2576,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="zone2200@hotmail.fr" refreshedDate="45290.772366435187" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="40" xr:uid="{AFCF1F28-6623-410C-B191-5B03B90EFEB8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="pc" refreshedDate="45296.985604398149" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="40" xr:uid="{C6F1E3E7-B6D4-4B4C-9239-916F971FBEC6}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A2:C42" sheet="Qustion 1"/>
+    <worksheetSource ref="A2:C42" sheet="Question1"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Students" numFmtId="0">
@@ -2584,10 +2599,10 @@
         <s v="Brown"/>
         <s v="Dartmouth"/>
         <s v="Harvard"/>
-        <s v="Colombia"/>
+        <s v="Columbia"/>
         <s v="Cornell"/>
         <s v="Princeton"/>
-        <s v="Penn state"/>
+        <s v="Penn"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -2634,7 +2649,7 @@
   <r>
     <n v="173"/>
     <x v="0"/>
-    <x v="4"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="1355"/>
@@ -2669,7 +2684,7 @@
   <r>
     <n v="972"/>
     <x v="2"/>
-    <x v="7"/>
+    <x v="1"/>
   </r>
   <r>
     <n v="234"/>
@@ -2805,7 +2820,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{040A9DCC-AC2F-4220-9D42-2164DE5C0B56}" name="Tableau croisé dynamique1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6731CE6C-28EC-4C47-804E-E07D0B57BF82}" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -2819,19 +2834,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0">
-      <items count="9">
-        <item x="1"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="1"/>
@@ -2868,8 +2871,8 @@
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="Somme de Students" fld="0" baseField="0" baseItem="0"/>
-    <dataField name="Moyenne de Students2" fld="0" subtotal="average" baseField="1" baseItem="0"/>
+    <dataField name="Sum of Students" fld="0" baseField="0" baseItem="0"/>
+    <dataField name="Average of Students2" fld="0" subtotal="average" baseField="1" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2884,7 +2887,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5A51970A-6A12-4A7C-8160-3664832D4D25}" name="Tableau croisé dynamique3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B5BB97F9-BA5D-4174-91ED-DE17EFB37EE5}" name="PivotTable3" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -2947,23 +2950,9 @@
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="Somme de Students" fld="0" baseField="0" baseItem="0"/>
-    <dataField name="Moyenne de Students2" fld="0" subtotal="average" baseField="2" baseItem="0"/>
+    <dataField name="Sum of Students" fld="0" baseField="0" baseItem="0"/>
+    <dataField name="Average of Students2" fld="0" subtotal="average" baseField="2" baseItem="0"/>
   </dataFields>
-  <formats count="1">
-    <format dxfId="0">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -2977,7 +2966,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2E074F0A-36CC-44CB-A1C4-25489CA510E1}" name="Tableau croisé dynamique4" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{15BC3064-5D30-4076-AF16-0A8039769E5A}" name="PivotTable4" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -3061,7 +3050,7 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Somme de Students" fld="0" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Students" fld="0" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -3076,7 +3065,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3371,231 +3360,575 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D62382-3F0C-47B1-8C75-BD9D67E59BAA}">
-  <dimension ref="A3:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046D4A60-888F-4140-8F0A-FF85C8B9EB7A}">
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="26">
+        <v>591</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7">
-        <v>8177</v>
-      </c>
-      <c r="C4" s="7">
-        <v>1022.125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="C3" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="27">
+        <v>9567</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="26">
+        <v>542</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
-        <v>4877</v>
-      </c>
-      <c r="C5" s="7">
-        <v>609.625</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="C5" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="27">
+        <v>346</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="26">
+        <v>849</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="27">
+        <v>552</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="26">
+        <v>173</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="27">
+        <v>1355</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="26">
+        <v>193</v>
+      </c>
+      <c r="B11" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
-        <v>7761</v>
-      </c>
-      <c r="C6" s="7">
-        <v>970.125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="C11" s="26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="27">
+        <v>615</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="26">
+        <v>1579</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="27">
+        <v>547</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="7">
-        <v>15071</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1883.875</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="C14" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="26">
+        <v>1687</v>
+      </c>
+      <c r="B15" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="7">
-        <v>4188</v>
-      </c>
-      <c r="C8" s="7">
-        <v>523.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="7">
-        <v>40074</v>
-      </c>
-      <c r="C9" s="7">
-        <v>1001.85</v>
+      <c r="C15" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="27">
+        <v>972</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="26">
+        <v>234</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="27">
+        <v>151</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="26">
+        <v>1793</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="27">
+        <v>315</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="26">
+        <v>618</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="27">
+        <v>246</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="26">
+        <v>784</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="27">
+        <v>316</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="26">
+        <v>3155</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="27">
+        <v>318</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="26">
+        <v>608</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="27">
+        <v>561</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="26">
+        <v>357</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="27">
+        <v>1688</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="26">
+        <v>972</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="27">
+        <v>568</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="26">
+        <v>632</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="27">
+        <v>551</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="26">
+        <v>948</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="27">
+        <v>1358</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="26">
+        <v>135</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="27">
+        <v>849</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="26">
+        <v>158</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="27">
+        <v>1889</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="26">
+        <v>651</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="27">
+        <v>651</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047C2E64-96F8-4D9F-A087-DD74FB44BD1F}">
-  <dimension ref="A3:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F09514-8AEA-4620-BF13-1AB3D12B013B}">
+  <dimension ref="A3:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="7">
-        <v>13155</v>
-      </c>
-      <c r="C4" s="8">
-        <v>3288.75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="7">
-        <v>5426</v>
-      </c>
-      <c r="C5" s="7">
-        <v>904.33333333333337</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="7">
-        <v>4965</v>
-      </c>
-      <c r="C6" s="7">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="7">
-        <v>6247</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1249.4000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="7">
-        <v>2067</v>
-      </c>
-      <c r="C8" s="7">
-        <v>516.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="7">
-        <v>2859</v>
-      </c>
-      <c r="C9" s="7">
-        <v>476.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="7">
-        <v>2661</v>
-      </c>
-      <c r="C10" s="7">
-        <v>532.20000000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="7">
-        <v>2694</v>
-      </c>
-      <c r="C11" s="7">
-        <v>538.79999999999995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="7">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="28">
+        <v>8177</v>
+      </c>
+      <c r="C4" s="28">
+        <v>1022.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="28">
+        <v>4877</v>
+      </c>
+      <c r="C5" s="28">
+        <v>609.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="28">
+        <v>7761</v>
+      </c>
+      <c r="C6" s="28">
+        <v>970.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="28">
+        <v>15071</v>
+      </c>
+      <c r="C7" s="28">
+        <v>1883.875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="28">
+        <v>4188</v>
+      </c>
+      <c r="C8" s="28">
+        <v>523.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="28">
         <v>40074</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C9" s="28">
         <v>1001.85</v>
       </c>
     </row>
@@ -3605,256 +3938,128 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB2FE21-229C-4764-B8B9-2B2C472D3852}">
-  <dimension ref="A3:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40E1D21-E077-4763-B2AD-DD9ECA756EA4}">
+  <dimension ref="A3:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7">
-        <v>1358</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7">
-        <v>1579</v>
-      </c>
-      <c r="E5" s="7">
-        <v>9567</v>
-      </c>
-      <c r="F5" s="7">
-        <v>651</v>
-      </c>
-      <c r="G5" s="7">
-        <v>13155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="B4" s="28">
+        <v>14127</v>
+      </c>
+      <c r="C4" s="28">
+        <v>2825.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="28">
+        <v>5253</v>
+      </c>
+      <c r="C5" s="28">
+        <v>1050.5999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="28">
+        <v>4965</v>
+      </c>
+      <c r="C6" s="28">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="28">
+        <v>6247</v>
+      </c>
+      <c r="C7" s="28">
+        <v>1249.4000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="28">
+        <v>2240</v>
+      </c>
+      <c r="C8" s="28">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="28">
+        <v>1887</v>
+      </c>
+      <c r="C9" s="28">
+        <v>377.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="7">
-        <v>1022</v>
-      </c>
-      <c r="C6" s="7">
-        <v>608</v>
-      </c>
-      <c r="D6" s="7">
-        <v>1688</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1793</v>
-      </c>
-      <c r="F6" s="7">
-        <v>315</v>
-      </c>
-      <c r="G6" s="7">
-        <v>5426</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7">
-        <v>1355</v>
-      </c>
-      <c r="C7" s="7">
-        <v>552</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1889</v>
-      </c>
-      <c r="E7" s="7">
-        <v>618</v>
-      </c>
-      <c r="F7" s="7">
-        <v>551</v>
-      </c>
-      <c r="G7" s="7">
-        <v>4965</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7">
-        <v>3155</v>
-      </c>
-      <c r="C8" s="7">
-        <v>542</v>
-      </c>
-      <c r="D8" s="7">
-        <v>316</v>
-      </c>
-      <c r="E8" s="7">
-        <v>547</v>
-      </c>
-      <c r="F8" s="7">
-        <v>1687</v>
-      </c>
-      <c r="G8" s="7">
-        <v>6247</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7">
-        <v>346</v>
-      </c>
-      <c r="D9" s="7">
-        <v>615</v>
-      </c>
-      <c r="E9" s="7">
-        <v>948</v>
-      </c>
-      <c r="F9" s="7">
-        <v>158</v>
-      </c>
-      <c r="G9" s="7">
-        <v>2067</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="7">
-        <v>135</v>
-      </c>
-      <c r="C10" s="7">
-        <v>1206</v>
-      </c>
-      <c r="D10" s="7">
-        <v>632</v>
-      </c>
-      <c r="E10" s="7">
-        <v>568</v>
-      </c>
-      <c r="F10" s="7">
-        <v>318</v>
-      </c>
-      <c r="G10" s="7">
-        <v>2859</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="7">
-        <v>561</v>
-      </c>
-      <c r="C11" s="7">
-        <v>972</v>
-      </c>
-      <c r="D11" s="7">
-        <v>193</v>
-      </c>
-      <c r="E11" s="7">
-        <v>784</v>
-      </c>
-      <c r="F11" s="7">
-        <v>151</v>
-      </c>
-      <c r="G11" s="7">
+      <c r="B10" s="28">
         <v>2661</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="C10" s="28">
+        <v>532.20000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="7">
-        <v>591</v>
-      </c>
-      <c r="C12" s="7">
-        <v>651</v>
-      </c>
-      <c r="D12" s="7">
-        <v>849</v>
-      </c>
-      <c r="E12" s="7">
-        <v>246</v>
-      </c>
-      <c r="F12" s="7">
-        <v>357</v>
-      </c>
-      <c r="G12" s="7">
+      <c r="B11" s="28">
         <v>2694</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="7">
-        <v>8177</v>
-      </c>
-      <c r="C13" s="7">
-        <v>4877</v>
-      </c>
-      <c r="D13" s="7">
-        <v>7761</v>
-      </c>
-      <c r="E13" s="7">
-        <v>15071</v>
-      </c>
-      <c r="F13" s="7">
-        <v>4188</v>
-      </c>
-      <c r="G13" s="7">
+      <c r="C11" s="28">
+        <v>538.79999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="28">
         <v>40074</v>
+      </c>
+      <c r="C12" s="28">
+        <v>1001.85</v>
       </c>
     </row>
   </sheetData>
@@ -3863,6 +4068,268 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7BE166-1392-4567-88CB-DE7EB31278D8}">
+  <dimension ref="A3:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="28">
+        <v>1358</v>
+      </c>
+      <c r="C5" s="28">
+        <v>972</v>
+      </c>
+      <c r="D5" s="28">
+        <v>1579</v>
+      </c>
+      <c r="E5" s="28">
+        <v>9567</v>
+      </c>
+      <c r="F5" s="28">
+        <v>651</v>
+      </c>
+      <c r="G5" s="28">
+        <v>14127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="28">
+        <v>849</v>
+      </c>
+      <c r="C6" s="28">
+        <v>608</v>
+      </c>
+      <c r="D6" s="28">
+        <v>1688</v>
+      </c>
+      <c r="E6" s="28">
+        <v>1793</v>
+      </c>
+      <c r="F6" s="28">
+        <v>315</v>
+      </c>
+      <c r="G6" s="28">
+        <v>5253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="28">
+        <v>1355</v>
+      </c>
+      <c r="C7" s="28">
+        <v>552</v>
+      </c>
+      <c r="D7" s="28">
+        <v>1889</v>
+      </c>
+      <c r="E7" s="28">
+        <v>618</v>
+      </c>
+      <c r="F7" s="28">
+        <v>551</v>
+      </c>
+      <c r="G7" s="28">
+        <v>4965</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="28">
+        <v>3155</v>
+      </c>
+      <c r="C8" s="28">
+        <v>542</v>
+      </c>
+      <c r="D8" s="28">
+        <v>316</v>
+      </c>
+      <c r="E8" s="28">
+        <v>547</v>
+      </c>
+      <c r="F8" s="28">
+        <v>1687</v>
+      </c>
+      <c r="G8" s="28">
+        <v>6247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="28">
+        <v>173</v>
+      </c>
+      <c r="C9" s="28">
+        <v>346</v>
+      </c>
+      <c r="D9" s="28">
+        <v>615</v>
+      </c>
+      <c r="E9" s="28">
+        <v>948</v>
+      </c>
+      <c r="F9" s="28">
+        <v>158</v>
+      </c>
+      <c r="G9" s="28">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="28">
+        <v>135</v>
+      </c>
+      <c r="C10" s="28">
+        <v>234</v>
+      </c>
+      <c r="D10" s="28">
+        <v>632</v>
+      </c>
+      <c r="E10" s="28">
+        <v>568</v>
+      </c>
+      <c r="F10" s="28">
+        <v>318</v>
+      </c>
+      <c r="G10" s="28">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="28">
+        <v>561</v>
+      </c>
+      <c r="C11" s="28">
+        <v>972</v>
+      </c>
+      <c r="D11" s="28">
+        <v>193</v>
+      </c>
+      <c r="E11" s="28">
+        <v>784</v>
+      </c>
+      <c r="F11" s="28">
+        <v>151</v>
+      </c>
+      <c r="G11" s="28">
+        <v>2661</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="28">
+        <v>591</v>
+      </c>
+      <c r="C12" s="28">
+        <v>651</v>
+      </c>
+      <c r="D12" s="28">
+        <v>849</v>
+      </c>
+      <c r="E12" s="28">
+        <v>246</v>
+      </c>
+      <c r="F12" s="28">
+        <v>357</v>
+      </c>
+      <c r="G12" s="28">
+        <v>2694</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="28">
+        <v>8177</v>
+      </c>
+      <c r="C13" s="28">
+        <v>4877</v>
+      </c>
+      <c r="D13" s="28">
+        <v>7761</v>
+      </c>
+      <c r="E13" s="28">
+        <v>15071</v>
+      </c>
+      <c r="F13" s="28">
+        <v>4188</v>
+      </c>
+      <c r="G13" s="28">
+        <v>40074</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B5A3E9-637D-4E95-A8C0-F8077A5ED135}">
   <dimension ref="A1:G21"/>
   <sheetViews>
@@ -3870,452 +4337,452 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="7"/>
-    <col min="4" max="4" width="16" style="11" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="1"/>
+    <col min="4" max="4" width="16" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="5">
         <v>120</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="3">
         <f>C2*B2</f>
         <v>360</v>
       </c>
-      <c r="E2" s="14" t="str">
+      <c r="E2" s="7" t="str">
         <f>IF(((D2&gt;=100)*AND(D2&lt;=999)),"5%",IF(D2&gt;=1000,"10%","0%"))</f>
         <v>5%</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="3">
         <f>D2*E2</f>
         <v>18</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="3">
         <f>D2-F2</f>
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="10">
         <v>56</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="11">
         <v>5</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="12">
         <f t="shared" ref="D3:D15" si="0">C3*B3</f>
         <v>280</v>
       </c>
-      <c r="E3" s="20" t="str">
+      <c r="E3" s="13" t="str">
         <f>IF(((D3&gt;=100)*AND(D3&lt;=999)),"5%",IF(D3&gt;=1000,"10%","0%"))</f>
         <v>5%</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="12">
         <f t="shared" ref="F3:F15" si="1">D3*E3</f>
         <v>14</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="12">
         <f t="shared" ref="G3:G15" si="2">D3-F3</f>
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="5">
         <v>70</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="3">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="E4" s="14" t="str">
-        <f t="shared" ref="E3:E15" si="3">IF(((D4&gt;=100)*AND(D4&lt;=999)),"5%",IF(D4&gt;=1000,"10%","0%"))</f>
+      <c r="E4" s="7" t="str">
+        <f t="shared" ref="E4:E15" si="3">IF(((D4&gt;=100)*AND(D4&lt;=999)),"5%",IF(D4&gt;=1000,"10%","0%"))</f>
         <v>5%</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="3">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="3">
         <f t="shared" si="2"/>
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="10">
         <v>430</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="11">
         <v>7</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="12">
         <f t="shared" si="0"/>
         <v>3010</v>
       </c>
-      <c r="E5" s="20" t="str">
+      <c r="E5" s="13" t="str">
         <f t="shared" si="3"/>
         <v>10%</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="12">
         <f t="shared" si="1"/>
         <v>301</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="12">
         <f t="shared" si="2"/>
         <v>2709</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="5">
         <v>230</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="2">
         <v>23</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>5290</v>
       </c>
-      <c r="E6" s="14" t="str">
+      <c r="E6" s="7" t="str">
         <f t="shared" si="3"/>
         <v>10%</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="3">
         <f t="shared" si="1"/>
         <v>529</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="3">
         <f t="shared" si="2"/>
         <v>4761</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="10">
         <v>10</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="11">
         <v>2</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="12">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E7" s="20" t="str">
+      <c r="E7" s="13" t="str">
         <f t="shared" si="3"/>
         <v>0%</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="12">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="2">
         <v>8</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E8" s="14" t="str">
+      <c r="E8" s="7" t="str">
         <f t="shared" si="3"/>
         <v>0%</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="3">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="10">
         <v>5040</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="11">
         <v>1</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="12">
         <f t="shared" si="0"/>
         <v>5040</v>
       </c>
-      <c r="E9" s="20" t="str">
+      <c r="E9" s="13" t="str">
         <f t="shared" si="3"/>
         <v>10%</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="12">
         <f t="shared" si="1"/>
         <v>504</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="12">
         <f t="shared" si="2"/>
         <v>4536</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="5">
         <v>1200</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="2">
         <v>3</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>3600</v>
       </c>
-      <c r="E10" s="14" t="str">
+      <c r="E10" s="7" t="str">
         <f t="shared" si="3"/>
         <v>10%</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="3">
         <f t="shared" si="1"/>
         <v>360</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="3">
         <f t="shared" si="2"/>
         <v>3240</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="10">
         <v>480</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="11">
         <v>4</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="12">
         <f t="shared" si="0"/>
         <v>1920</v>
       </c>
-      <c r="E11" s="20" t="str">
+      <c r="E11" s="13" t="str">
         <f t="shared" si="3"/>
         <v>10%</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="12">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="12">
         <f t="shared" si="2"/>
         <v>1728</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="5">
         <v>33</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="2">
         <v>5</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
         <v>165</v>
       </c>
-      <c r="E12" s="14" t="str">
+      <c r="E12" s="7" t="str">
         <f t="shared" si="3"/>
         <v>5%</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="3">
         <f t="shared" si="1"/>
         <v>8.25</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="3">
         <f t="shared" si="2"/>
         <v>156.75</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="10">
         <v>1200</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="11">
         <v>2</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="12">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
-      <c r="E13" s="20" t="str">
+      <c r="E13" s="13" t="str">
         <f t="shared" si="3"/>
         <v>10%</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="12">
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="12">
         <f t="shared" si="2"/>
         <v>2160</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="5">
         <v>15</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="2">
         <v>10</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="3">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="E14" s="14" t="str">
+      <c r="E14" s="7" t="str">
         <f t="shared" si="3"/>
         <v>5%</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="3">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="3">
         <f t="shared" si="2"/>
         <v>142.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
         <v>14</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="10">
         <v>24</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="11">
         <v>5</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="12">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E15" s="20" t="str">
+      <c r="E15" s="13" t="str">
         <f t="shared" si="3"/>
         <v>5%</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="12">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="12">
         <f t="shared" si="2"/>
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E18" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="10">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E18" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="3">
         <f>SUM(G2:G15)</f>
         <v>20348.25</v>
       </c>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E19" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="28">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E19" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="19">
         <v>0.19</v>
       </c>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="10">
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="3">
         <f>(SUM(G2:G15)*G19)/100%</f>
         <v>3866.1675</v>
       </c>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="19">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E21" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="12">
         <f>G18+G20</f>
         <v>24214.4175</v>
       </c>
@@ -4331,7 +4798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB74F61-3D7D-415D-9ED8-BA8191AED5B7}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -4339,139 +4806,139 @@
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="1" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="8">
         <v>5</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="8">
         <f>B2/A2</f>
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="9">
         <v>10</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="9">
         <f t="shared" ref="C3:C11" si="0">B3/A3</f>
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="8">
         <v>17</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="8">
         <f t="shared" si="0"/>
         <v>5.666666666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="9">
         <v>17</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="9">
         <f t="shared" si="0"/>
         <v>4.25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="8">
         <v>37</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="8">
         <f t="shared" si="0"/>
         <v>7.4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="9">
         <v>49</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="9">
         <f t="shared" si="0"/>
         <v>8.1666666666666661</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="8">
         <v>63</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="8">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="9">
         <v>75</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="9">
         <f t="shared" si="0"/>
         <v>9.375</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="8">
         <v>83</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="8">
         <f t="shared" si="0"/>
         <v>9.2222222222222214</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="9">
         <v>91</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="9">
         <f t="shared" si="0"/>
         <v>9.1</v>
       </c>
@@ -4480,485 +4947,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF5D96D-FA04-4556-9F7E-5244211C2588}">
-  <dimension ref="A1:C42"/>
-  <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>591</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>9567</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>542</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>346</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>849</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>552</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>173</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>1355</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>193</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>615</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>1579</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>547</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>1687</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>972</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>234</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>151</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>1793</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>315</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>618</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>246</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>784</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>316</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>3155</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>318</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>608</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>561</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>357</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>1688</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>972</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>568</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>632</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>551</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>948</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>1358</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>135</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>849</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>158</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>1889</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <v>651</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>651</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>